<commit_message>
4 mdelo melhores rstds
</commit_message>
<xml_diff>
--- a/2024/nuno-dataset/test-oxigen/content/results/metrics_10_0.xlsx
+++ b/2024/nuno-dataset/test-oxigen/content/results/metrics_10_0.xlsx
@@ -478,32 +478,32 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>model_10_0_17</t>
+          <t>model_10_0_0</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.4731349088542739</v>
+        <v>0.419820259694951</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.7001773799608941</v>
+        <v>0.1508400527664997</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.8622199637366839</v>
+        <v>0.06568731025436791</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.8236206841842182</v>
+        <v>0.3255605975328584</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5830844044685364</v>
+        <v>0.6420879364013672</v>
       </c>
       <c r="G2" t="n">
-        <v>0.7981682419776917</v>
+        <v>1.730097413063049</v>
       </c>
       <c r="H2" t="n">
-        <v>3.15552020072937</v>
+        <v>0.2272701263427734</v>
       </c>
       <c r="I2" t="n">
-        <v>1.907509803771973</v>
+        <v>1.022884607315063</v>
       </c>
     </row>
     <row r="3">
@@ -513,121 +513,121 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.5036784631811615</v>
+        <v>0.4969228240677905</v>
       </c>
       <c r="C3" t="n">
-        <v>-1.24275654423519</v>
+        <v>-0.2396846936711678</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.5568266158090438</v>
+        <v>-2.958831824791341</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.7197300823802799</v>
+        <v>-0.1804578123918912</v>
       </c>
       <c r="F3" t="n">
-        <v>0.5492816567420959</v>
+        <v>0.5567582249641418</v>
       </c>
       <c r="G3" t="n">
-        <v>1.0528883934021</v>
+        <v>2.525761365890503</v>
       </c>
       <c r="H3" t="n">
-        <v>2.638032913208008</v>
+        <v>0.9629797339439392</v>
       </c>
       <c r="I3" t="n">
-        <v>1.798840165138245</v>
+        <v>1.790334582328796</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>model_10_0_21</t>
+          <t>model_10_0_23</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.508459012273401</v>
+        <v>0.4992061052142013</v>
       </c>
       <c r="C4" t="n">
-        <v>-1.088824271965264</v>
+        <v>-0.2335032557486374</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.5827694606463532</v>
+        <v>-2.943191963401899</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.70292934068517</v>
+        <v>-0.1748807793798524</v>
       </c>
       <c r="F4" t="n">
-        <v>0.5439910292625427</v>
+        <v>0.5542313456535339</v>
       </c>
       <c r="G4" t="n">
-        <v>0.9806230068206787</v>
+        <v>2.513166904449463</v>
       </c>
       <c r="H4" t="n">
-        <v>2.681993007659912</v>
+        <v>0.9591754078865051</v>
       </c>
       <c r="I4" t="n">
-        <v>1.781266450881958</v>
+        <v>1.7818763256073</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>model_10_0_23</t>
+          <t>model_10_0_22</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.5086700346262356</v>
+        <v>0.4999152102463791</v>
       </c>
       <c r="C5" t="n">
-        <v>-1.177722642390179</v>
+        <v>-0.2335783442883954</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.5542295448236478</v>
+        <v>-2.916870107171301</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.7022963898468477</v>
+        <v>-0.172948193177267</v>
       </c>
       <c r="F5" t="n">
-        <v>0.5437574982643127</v>
+        <v>0.5534464716911316</v>
       </c>
       <c r="G5" t="n">
-        <v>1.02235746383667</v>
+        <v>2.513319969177246</v>
       </c>
       <c r="H5" t="n">
-        <v>2.633632183074951</v>
+        <v>0.9527726173400879</v>
       </c>
       <c r="I5" t="n">
-        <v>1.780604362487793</v>
+        <v>1.778945207595825</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>model_10_0_22</t>
+          <t>model_10_0_21</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.509169374439546</v>
+        <v>0.5148962607036258</v>
       </c>
       <c r="C6" t="n">
-        <v>-1.132604363591517</v>
+        <v>-0.1824374153236399</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.5659543033291488</v>
+        <v>-2.921112719552709</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.7005122598469449</v>
+        <v>-0.1368967211696703</v>
       </c>
       <c r="F6" t="n">
-        <v>0.5432048439979553</v>
+        <v>0.5368668437004089</v>
       </c>
       <c r="G6" t="n">
-        <v>1.001176238059998</v>
+        <v>2.409124374389648</v>
       </c>
       <c r="H6" t="n">
-        <v>2.653499603271484</v>
+        <v>0.9538046717643738</v>
       </c>
       <c r="I6" t="n">
-        <v>1.778738260269165</v>
+        <v>1.724268078804016</v>
       </c>
     </row>
     <row r="7">
@@ -637,28 +637,28 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.5105627637855117</v>
+        <v>0.5164138484376217</v>
       </c>
       <c r="C7" t="n">
-        <v>-1.042024182422857</v>
+        <v>-0.1865260207426036</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.5876658029762363</v>
+        <v>-2.832788886300593</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.6955440482626747</v>
+        <v>-0.1331381778284531</v>
       </c>
       <c r="F7" t="n">
-        <v>0.5416628122329712</v>
+        <v>0.5351873636245728</v>
       </c>
       <c r="G7" t="n">
-        <v>0.9586522579193115</v>
+        <v>2.417454481124878</v>
       </c>
       <c r="H7" t="n">
-        <v>2.690289974212646</v>
+        <v>0.9323199987411499</v>
       </c>
       <c r="I7" t="n">
-        <v>1.773541450500488</v>
+        <v>1.718567490577698</v>
       </c>
     </row>
     <row r="8">
@@ -668,152 +668,152 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.5115686400358618</v>
+        <v>0.5276554921772456</v>
       </c>
       <c r="C8" t="n">
-        <v>-1.018736686743969</v>
+        <v>-0.1470391388140471</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.5902876039195089</v>
+        <v>-2.844337142768619</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.692006367719386</v>
+        <v>-0.105927266958471</v>
       </c>
       <c r="F8" t="n">
-        <v>0.5405495762825012</v>
+        <v>0.522746205329895</v>
       </c>
       <c r="G8" t="n">
-        <v>0.9477196931838989</v>
+        <v>2.337003231048584</v>
       </c>
       <c r="H8" t="n">
-        <v>2.694732666015625</v>
+        <v>0.9351291656494141</v>
       </c>
       <c r="I8" t="n">
-        <v>1.769841194152832</v>
+        <v>1.677298307418823</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>model_10_0_18</t>
+          <t>model_10_0_1</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.5127913612913917</v>
+        <v>0.5288798698710702</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.9450474155352149</v>
+        <v>0.3189295441339353</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.607471718997658</v>
+        <v>-1.096691514476998</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.6876013016335456</v>
+        <v>0.357374229522472</v>
       </c>
       <c r="F9" t="n">
-        <v>0.5391964316368103</v>
+        <v>0.5213912129402161</v>
       </c>
       <c r="G9" t="n">
-        <v>0.9131253361701965</v>
+        <v>1.387628078460693</v>
       </c>
       <c r="H9" t="n">
-        <v>2.723850965499878</v>
+        <v>0.5100170373916626</v>
       </c>
       <c r="I9" t="n">
-        <v>1.765233278274536</v>
+        <v>0.9746347069740295</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>model_10_0_16</t>
+          <t>model_10_0_18</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.5200906903552422</v>
+        <v>0.5380671359296699</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.4351091212996387</v>
+        <v>-0.1128822278538824</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.7273713650163875</v>
+        <v>-2.832536775327245</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.6578343756765572</v>
+        <v>-0.08074372548928932</v>
       </c>
       <c r="F10" t="n">
-        <v>0.5311182737350464</v>
+        <v>0.5112235546112061</v>
       </c>
       <c r="G10" t="n">
-        <v>0.6737288236618042</v>
+        <v>2.267411231994629</v>
       </c>
       <c r="H10" t="n">
-        <v>2.927020072937012</v>
+        <v>0.9322587251663208</v>
       </c>
       <c r="I10" t="n">
-        <v>1.734097123146057</v>
+        <v>1.639103889465332</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>model_10_0_0</t>
+          <t>model_10_0_17</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.5518903425399277</v>
+        <v>0.562202191296568</v>
       </c>
       <c r="C11" t="n">
-        <v>0.2476780459984151</v>
+        <v>-0.04911300738385549</v>
       </c>
       <c r="D11" t="n">
-        <v>0.315351368063297</v>
+        <v>-2.662741530402664</v>
       </c>
       <c r="E11" t="n">
-        <v>0.2993070850448647</v>
+        <v>-0.02257554747442869</v>
       </c>
       <c r="F11" t="n">
-        <v>0.4959253668785095</v>
+        <v>0.484513133764267</v>
       </c>
       <c r="G11" t="n">
-        <v>0.3531863987445831</v>
+        <v>2.137486219406128</v>
       </c>
       <c r="H11" t="n">
-        <v>1.160132884979248</v>
+        <v>0.8909562826156616</v>
       </c>
       <c r="I11" t="n">
-        <v>0.7329257726669312</v>
+        <v>1.550883412361145</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>model_10_0_1</t>
+          <t>model_10_0_16</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.594758446783998</v>
+        <v>0.5819404989476881</v>
       </c>
       <c r="C12" t="n">
-        <v>0.4919952997244803</v>
+        <v>0.0225000566697432</v>
       </c>
       <c r="D12" t="n">
-        <v>0.2425684894444124</v>
+        <v>-2.70260807979344</v>
       </c>
       <c r="E12" t="n">
-        <v>0.30187347743054</v>
+        <v>0.0253464196535591</v>
       </c>
       <c r="F12" t="n">
-        <v>0.4484829902648926</v>
+        <v>0.4626686871051788</v>
       </c>
       <c r="G12" t="n">
-        <v>0.2384887486696243</v>
+        <v>1.991580128669739</v>
       </c>
       <c r="H12" t="n">
-        <v>1.283463001251221</v>
+        <v>0.9006537199020386</v>
       </c>
       <c r="I12" t="n">
-        <v>0.7302412986755371</v>
+        <v>1.478202819824219</v>
       </c>
     </row>
     <row r="13">
@@ -823,431 +823,431 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.649318921793276</v>
+        <v>0.5970848982712313</v>
       </c>
       <c r="C13" t="n">
-        <v>0.08011774881133282</v>
+        <v>0.0727302707069174</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.2955542797510913</v>
+        <v>-2.681978615969077</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.2062264614823028</v>
+        <v>0.06262677344953438</v>
       </c>
       <c r="F13" t="n">
-        <v>0.3881006240844727</v>
+        <v>0.4459083080291748</v>
       </c>
       <c r="G13" t="n">
-        <v>0.4318495392799377</v>
+        <v>1.889240026473999</v>
       </c>
       <c r="H13" t="n">
-        <v>2.195308685302734</v>
+        <v>0.8956356048583984</v>
       </c>
       <c r="I13" t="n">
-        <v>1.261714577674866</v>
+        <v>1.421661853790283</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>model_10_0_2</t>
+          <t>model_10_0_14</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.6978130705938026</v>
+        <v>0.6027181045287496</v>
       </c>
       <c r="C14" t="n">
-        <v>0.7044614528960115</v>
+        <v>0.09024114193297916</v>
       </c>
       <c r="D14" t="n">
-        <v>0.1701671407602806</v>
+        <v>-2.667080148839596</v>
       </c>
       <c r="E14" t="n">
-        <v>0.2971629041152235</v>
+        <v>0.0762048460567204</v>
       </c>
       <c r="F14" t="n">
-        <v>0.3344318568706512</v>
+        <v>0.4396739900112152</v>
       </c>
       <c r="G14" t="n">
-        <v>0.138744056224823</v>
+        <v>1.853562831878662</v>
       </c>
       <c r="H14" t="n">
-        <v>1.40614652633667</v>
+        <v>0.8920116424560547</v>
       </c>
       <c r="I14" t="n">
-        <v>0.7351685762405396</v>
+        <v>1.401068687438965</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>model_10_0_3</t>
+          <t>model_10_0_13</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.706012493649376</v>
+        <v>0.6670572757386747</v>
       </c>
       <c r="C15" t="n">
-        <v>0.7058040683027376</v>
+        <v>0.3073390224649396</v>
       </c>
       <c r="D15" t="n">
-        <v>0.1767029716323895</v>
+        <v>-2.651357946646561</v>
       </c>
       <c r="E15" t="n">
-        <v>0.3024646197417571</v>
+        <v>0.2317914741168796</v>
       </c>
       <c r="F15" t="n">
-        <v>0.3253574967384338</v>
+        <v>0.3684695065021515</v>
       </c>
       <c r="G15" t="n">
-        <v>0.1381137371063232</v>
+        <v>1.411242961883545</v>
       </c>
       <c r="H15" t="n">
-        <v>1.395071744918823</v>
+        <v>0.8881872296333313</v>
       </c>
       <c r="I15" t="n">
-        <v>0.729623019695282</v>
+        <v>1.165099143981934</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>model_10_0_4</t>
+          <t>model_10_0_12</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.7128577370715187</v>
+        <v>0.694459231713451</v>
       </c>
       <c r="C16" t="n">
-        <v>0.7072258243373033</v>
+        <v>0.4040199255396154</v>
       </c>
       <c r="D16" t="n">
-        <v>0.1852828857931038</v>
+        <v>-2.679648699860401</v>
       </c>
       <c r="E16" t="n">
-        <v>0.3093426111657697</v>
+        <v>0.2984154893126019</v>
       </c>
       <c r="F16" t="n">
-        <v>0.3177818655967712</v>
+        <v>0.3381435871124268</v>
       </c>
       <c r="G16" t="n">
-        <v>0.1374462693929672</v>
+        <v>1.214263081550598</v>
       </c>
       <c r="H16" t="n">
-        <v>1.3805330991745</v>
+        <v>0.8950689435005188</v>
       </c>
       <c r="I16" t="n">
-        <v>0.7224286198616028</v>
+        <v>1.064054131507874</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>model_10_0_14</t>
+          <t>model_10_0_11</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.7522123783474219</v>
+        <v>0.7068957371583571</v>
       </c>
       <c r="C17" t="n">
-        <v>0.2634170041326134</v>
+        <v>0.4752967080705121</v>
       </c>
       <c r="D17" t="n">
-        <v>0.1209714305054012</v>
+        <v>-2.93923054432014</v>
       </c>
       <c r="E17" t="n">
-        <v>0.1548621055621802</v>
+        <v>0.3295155634252815</v>
       </c>
       <c r="F17" t="n">
-        <v>0.2742278575897217</v>
+        <v>0.3243800699710846</v>
       </c>
       <c r="G17" t="n">
-        <v>0.3457975685596466</v>
+        <v>1.069042205810547</v>
       </c>
       <c r="H17" t="n">
-        <v>1.489508390426636</v>
+        <v>0.9582117795944214</v>
       </c>
       <c r="I17" t="n">
-        <v>0.8840155005455017</v>
+        <v>1.016886472702026</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>model_10_0_5</t>
+          <t>model_10_0_2</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.8014537951350098</v>
+        <v>0.7268433593104267</v>
       </c>
       <c r="C18" t="n">
-        <v>0.7574436774974571</v>
+        <v>0.5866644898789335</v>
       </c>
       <c r="D18" t="n">
-        <v>0.4257923769411776</v>
+        <v>-1.55057947113447</v>
       </c>
       <c r="E18" t="n">
-        <v>0.5046247381355256</v>
+        <v>0.5135294163953268</v>
       </c>
       <c r="F18" t="n">
-        <v>0.2197321504354477</v>
+        <v>0.3023039400577545</v>
       </c>
       <c r="G18" t="n">
-        <v>0.1138709113001823</v>
+        <v>0.8421390056610107</v>
       </c>
       <c r="H18" t="n">
-        <v>0.9729912877082825</v>
+        <v>0.6204245090484619</v>
       </c>
       <c r="I18" t="n">
-        <v>0.51816326379776</v>
+        <v>0.7378028631210327</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>model_10_0_13</t>
+          <t>model_10_0_10</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.8035700660473902</v>
+        <v>0.7352852167885662</v>
       </c>
       <c r="C19" t="n">
-        <v>0.3913522864483999</v>
+        <v>0.5749494530138082</v>
       </c>
       <c r="D19" t="n">
-        <v>0.3199864502773686</v>
+        <v>-2.956782391586033</v>
       </c>
       <c r="E19" t="n">
-        <v>0.3369786521194795</v>
+        <v>0.399063556320255</v>
       </c>
       <c r="F19" t="n">
-        <v>0.2173900604248047</v>
+        <v>0.2929612696170807</v>
       </c>
       <c r="G19" t="n">
-        <v>0.2857367992401123</v>
+        <v>0.8660074472427368</v>
       </c>
       <c r="H19" t="n">
-        <v>1.152278780937195</v>
+        <v>0.9624812006950378</v>
       </c>
       <c r="I19" t="n">
-        <v>0.69352126121521</v>
+        <v>0.911406934261322</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>model_10_0_6</t>
+          <t>model_10_0_9</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.8091066628302312</v>
+        <v>0.7365824728627355</v>
       </c>
       <c r="C20" t="n">
-        <v>0.696125918970782</v>
+        <v>0.5799447637082356</v>
       </c>
       <c r="D20" t="n">
-        <v>0.4752401841077747</v>
+        <v>-2.960262573006388</v>
       </c>
       <c r="E20" t="n">
-        <v>0.5277514673032757</v>
+        <v>0.4023534166901206</v>
       </c>
       <c r="F20" t="n">
-        <v>0.2112626731395721</v>
+        <v>0.2915255725383759</v>
       </c>
       <c r="G20" t="n">
-        <v>0.1426572352647781</v>
+        <v>0.8558299541473389</v>
       </c>
       <c r="H20" t="n">
-        <v>0.8892022371292114</v>
+        <v>0.9633278250694275</v>
       </c>
       <c r="I20" t="n">
-        <v>0.4939726591110229</v>
+        <v>0.9064173698425293</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>model_10_0_7</t>
+          <t>model_10_0_8</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.8133423256212595</v>
+        <v>0.7456997853790047</v>
       </c>
       <c r="C21" t="n">
-        <v>0.6056348927819581</v>
+        <v>0.6078428121162333</v>
       </c>
       <c r="D21" t="n">
-        <v>0.4222629711468249</v>
+        <v>-2.92992169844679</v>
       </c>
       <c r="E21" t="n">
-        <v>0.4658630738623734</v>
+        <v>0.4244843087619784</v>
       </c>
       <c r="F21" t="n">
-        <v>0.2065750360488892</v>
+        <v>0.2814354002475739</v>
       </c>
       <c r="G21" t="n">
-        <v>0.1851393431425095</v>
+        <v>0.7989897727966309</v>
       </c>
       <c r="H21" t="n">
-        <v>0.9789718389511108</v>
+        <v>0.9559473991394043</v>
       </c>
       <c r="I21" t="n">
-        <v>0.5587079524993896</v>
+        <v>0.8728526830673218</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>model_10_0_8</t>
+          <t>model_10_0_7</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.8181657943074527</v>
+        <v>0.7472548583392919</v>
       </c>
       <c r="C22" t="n">
-        <v>0.4908372992091166</v>
+        <v>0.6105217449131943</v>
       </c>
       <c r="D22" t="n">
-        <v>0.3952329316424759</v>
+        <v>-2.902218420987799</v>
       </c>
       <c r="E22" t="n">
-        <v>0.4179807749656536</v>
+        <v>0.4284807020312199</v>
       </c>
       <c r="F22" t="n">
-        <v>0.2012368887662888</v>
+        <v>0.2797144055366516</v>
       </c>
       <c r="G22" t="n">
-        <v>0.2390324026346207</v>
+        <v>0.7935316562652588</v>
       </c>
       <c r="H22" t="n">
-        <v>1.024774074554443</v>
+        <v>0.949208676815033</v>
       </c>
       <c r="I22" t="n">
-        <v>0.6087929606437683</v>
+        <v>0.8667914867401123</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>model_10_0_9</t>
+          <t>model_10_0_6</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.8218188418480434</v>
+        <v>0.7665514841132238</v>
       </c>
       <c r="C23" t="n">
-        <v>0.490766429440429</v>
+        <v>0.6550190178298698</v>
       </c>
       <c r="D23" t="n">
-        <v>0.3946831489748902</v>
+        <v>-2.676953969625329</v>
       </c>
       <c r="E23" t="n">
-        <v>0.4175443165737779</v>
+        <v>0.4771292039649689</v>
       </c>
       <c r="F23" t="n">
-        <v>0.1971940547227859</v>
+        <v>0.2583587169647217</v>
       </c>
       <c r="G23" t="n">
-        <v>0.2390656471252441</v>
+        <v>0.7028719782829285</v>
       </c>
       <c r="H23" t="n">
-        <v>1.025705575942993</v>
+        <v>0.8944134116172791</v>
       </c>
       <c r="I23" t="n">
-        <v>0.6092495322227478</v>
+        <v>0.7930090427398682</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>model_10_0_12</t>
+          <t>model_10_0_5</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.8233333904905971</v>
+        <v>0.7816042624276021</v>
       </c>
       <c r="C24" t="n">
-        <v>0.4290038765949785</v>
+        <v>0.691639924214684</v>
       </c>
       <c r="D24" t="n">
-        <v>0.4026124858328527</v>
+        <v>-2.494555289977589</v>
       </c>
       <c r="E24" t="n">
-        <v>0.4089139999507385</v>
+        <v>0.5169405941608965</v>
       </c>
       <c r="F24" t="n">
-        <v>0.1955178678035736</v>
+        <v>0.2416997104883194</v>
       </c>
       <c r="G24" t="n">
-        <v>0.2680608332157135</v>
+        <v>0.6282597184181213</v>
       </c>
       <c r="H24" t="n">
-        <v>1.012269377708435</v>
+        <v>0.8500452041625977</v>
       </c>
       <c r="I24" t="n">
-        <v>0.618276834487915</v>
+        <v>0.7326292991638184</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>model_10_0_10</t>
+          <t>model_10_0_3</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.8236312591678614</v>
+        <v>0.7867403416251588</v>
       </c>
       <c r="C25" t="n">
-        <v>0.4486570944556535</v>
+        <v>0.7112173110684303</v>
       </c>
       <c r="D25" t="n">
-        <v>0.4119181275435142</v>
+        <v>-1.788497607859882</v>
       </c>
       <c r="E25" t="n">
-        <v>0.420678375303701</v>
+        <v>0.5841542122836794</v>
       </c>
       <c r="F25" t="n">
-        <v>0.1951882094144821</v>
+        <v>0.2360156029462814</v>
       </c>
       <c r="G25" t="n">
-        <v>0.2588343918323517</v>
+        <v>0.5883723497390747</v>
       </c>
       <c r="H25" t="n">
-        <v>0.9965010285377502</v>
+        <v>0.6782978177070618</v>
       </c>
       <c r="I25" t="n">
-        <v>0.6059712767601013</v>
+        <v>0.6306900978088379</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>model_10_0_11</t>
+          <t>model_10_0_4</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.824243212624904</v>
+        <v>0.7915050457831647</v>
       </c>
       <c r="C26" t="n">
-        <v>0.418841236348467</v>
+        <v>0.7106854003209669</v>
       </c>
       <c r="D26" t="n">
-        <v>0.4132400022285554</v>
+        <v>-2.205712927260333</v>
       </c>
       <c r="E26" t="n">
-        <v>0.4146012369762806</v>
+        <v>0.5522861803255941</v>
       </c>
       <c r="F26" t="n">
-        <v>0.1945109665393829</v>
+        <v>0.230742484331131</v>
       </c>
       <c r="G26" t="n">
-        <v>0.2728317975997925</v>
+        <v>0.5894560217857361</v>
       </c>
       <c r="H26" t="n">
-        <v>0.9942611455917358</v>
+        <v>0.7797847986221313</v>
       </c>
       <c r="I26" t="n">
-        <v>0.6123279333114624</v>
+        <v>0.6790226697921753</v>
       </c>
     </row>
   </sheetData>

</xml_diff>